<commit_message>
update to list of accounts
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/CRB.xlsx
+++ b/aCCTg. pROGRAm/CRB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
   <si>
     <t>sCHEDULe</t>
   </si>
@@ -1429,11 +1429,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,20 +1783,18 @@
       <c r="F41" s="20"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>55</v>
+      <c r="A42" s="50" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
-        <v>102</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B43" s="20"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="B44" s="20"/>
+      <c r="B44" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>